<commit_message>
Merge 2 sorted arrays
</commit_message>
<xml_diff>
--- a/Love Babbar Sheet.xlsx
+++ b/Love Babbar Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Codes\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F33A4EC-ABB9-436F-9750-E373AA62B7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DC376D-78D6-4EE7-8C04-B3A4C462D027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="12549" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="468">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1421,6 +1421,9 @@
   </si>
   <si>
     <t>Power Set</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -1760,7 +1763,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.61328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1931,7 +1934,9 @@
       <c r="B17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="8"/>
+      <c r="C17" s="8" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="6" t="s">

</xml_diff>